<commit_message>
updated Array and Queue tests
</commit_message>
<xml_diff>
--- a/target/test-classes/TestData/dsAlgo_TestData.xlsx
+++ b/target/test-classes/TestData/dsAlgo_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimre\eclipse-workspace\DSAlgoTestNG_ClubNinjas\ClubNinjas_DsAlgoTestNG\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D083FD-7533-4751-B630-331013110158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9186A241-AA02-4767-A941-794D1FF1A526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="2" r:id="rId1"/>
@@ -2108,8 +2108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19390E6-AB14-4B31-A0B5-2F88190D0871}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2407,7 +2407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C156544-10E3-4CC6-B021-D85ABA7773B9}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>